<commit_message>
updated bwm and prem
</commit_message>
<xml_diff>
--- a/BWM/Vorlage_Ü2-14_Ü2-18.xlsx
+++ b/BWM/Vorlage_Ü2-14_Ü2-18.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\github_for_school\3DHIF_D_2025_26\BWM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF17FF4B-CD80-4E23-9FCB-3EED8C84EF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866843B-3E07-41E1-9A5A-5F956FBCDBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9D0B6A4D-E5E0-4723-A79C-6CA9A07D0E99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{9D0B6A4D-E5E0-4723-A79C-6CA9A07D0E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Ü 2.14" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
     <t>Ü 2.14 Kostenartenrechnung – Betriebsüberleitungsbogen</t>
   </si>
@@ -357,6 +357,57 @@
   </si>
   <si>
     <t>BGA</t>
+  </si>
+  <si>
+    <t>kalk. Zinsen</t>
+  </si>
+  <si>
+    <t>Ek:</t>
+  </si>
+  <si>
+    <t>Fk:</t>
+  </si>
+  <si>
+    <t>Summe:</t>
+  </si>
+  <si>
+    <t>kalk. Unternehmenrlohn:</t>
+  </si>
+  <si>
+    <t>p.a:</t>
+  </si>
+  <si>
+    <t>2. Quartal:</t>
+  </si>
+  <si>
+    <t>kalk. Unternehmenrlohn</t>
+  </si>
+  <si>
+    <t>kalk. Wagnisse</t>
+  </si>
+  <si>
+    <t>kalk. Wagnisse:</t>
+  </si>
+  <si>
+    <t>Vertriebsw:</t>
+  </si>
+  <si>
+    <t>Gewährleisungsw:</t>
+  </si>
+  <si>
+    <t>Anlage - Beständew:</t>
+  </si>
+  <si>
+    <t>weil</t>
+  </si>
+  <si>
+    <t>180000*0,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weil </t>
+  </si>
+  <si>
+    <t>254200*0,15</t>
   </si>
 </sst>
 </file>
@@ -798,46 +849,6 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -848,6 +859,46 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2005,48 +2056,48 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="59"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="58" t="s">
+      <c r="E5" s="66"/>
+      <c r="F5" s="65" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="58"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="58"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
@@ -2490,7 +2541,7 @@
         <v>183.2</v>
       </c>
       <c r="D30" s="28">
-        <f t="shared" ref="D30:F30" si="0">SUM(D7:D23)</f>
+        <f t="shared" ref="D30" si="0">SUM(D7:D23)</f>
         <v>44.599999999999994</v>
       </c>
       <c r="E30" s="28">
@@ -2530,7 +2581,7 @@
       <c r="B33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="61" t="s">
+      <c r="D33" s="50" t="s">
         <v>50</v>
       </c>
       <c r="E33" s="35" t="s">
@@ -2550,14 +2601,14 @@
       <c r="E34" s="35">
         <v>60000</v>
       </c>
-      <c r="F34" s="62"/>
+      <c r="F34" s="51"/>
       <c r="H34" s="35"/>
     </row>
     <row r="35" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D35" s="35">
         <v>60000</v>
       </c>
-      <c r="F35" s="62"/>
+      <c r="F35" s="51"/>
     </row>
     <row r="36" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="35" t="s">
@@ -2567,7 +2618,7 @@
         <f>D34-E34</f>
         <v>222500</v>
       </c>
-      <c r="E36" s="66" t="s">
+      <c r="E36" s="55" t="s">
         <v>53</v>
       </c>
       <c r="F36" s="35">
@@ -2584,7 +2635,7 @@
       <c r="G37" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H37" s="66" t="s">
+      <c r="H37" s="55" t="s">
         <v>59</v>
       </c>
       <c r="I37" s="4" t="s">
@@ -2592,17 +2643,17 @@
       </c>
     </row>
     <row r="38" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F38" s="65">
+      <c r="F38" s="54">
         <f>D36*(F36/F37)</f>
         <v>235214.28571428571</v>
       </c>
-      <c r="G38" s="66" t="s">
+      <c r="G38" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="H38" s="66">
+      <c r="H38" s="55">
         <v>8</v>
       </c>
-      <c r="I38" s="65">
+      <c r="I38" s="54">
         <f>F38/H38</f>
         <v>29401.785714285714</v>
       </c>
@@ -2633,10 +2684,10 @@
         <f>D40-D41</f>
         <v>265000</v>
       </c>
-      <c r="E42" s="66" t="s">
+      <c r="E42" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="F42" s="67">
+      <c r="F42" s="56">
         <v>265</v>
       </c>
       <c r="G42" s="35" t="s">
@@ -2644,28 +2695,28 @@
       </c>
     </row>
     <row r="43" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F43" s="67">
+      <c r="F43" s="56">
         <v>250</v>
       </c>
       <c r="G43" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H43" s="66" t="s">
+      <c r="H43" s="55" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F44" s="62">
+      <c r="F44" s="51">
         <f>D42*(F42/F43)</f>
         <v>280900</v>
       </c>
-      <c r="G44" s="66" t="s">
+      <c r="G44" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="H44" s="66">
+      <c r="H44" s="55">
         <v>10</v>
       </c>
-      <c r="I44" s="65">
+      <c r="I44" s="54">
         <f>F44/H44</f>
         <v>28090</v>
       </c>
@@ -2684,7 +2735,7 @@
       <c r="H48" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="I48" s="65">
+      <c r="I48" s="54">
         <f>I46+I44+I38</f>
         <v>269491.78571428574</v>
       </c>
@@ -2693,7 +2744,7 @@
       <c r="H49" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="I49" s="65">
+      <c r="I49" s="54">
         <f>I48/12</f>
         <v>22457.648809523813</v>
       </c>
@@ -3267,8 +3318,8 @@
   </sheetPr>
   <dimension ref="A1:H519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="121" zoomScaleNormal="115" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="M31" sqref="F31:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -3298,44 +3349,44 @@
       <c r="A3" s="37"/>
     </row>
     <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="59"/>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60" t="s">
+      <c r="E5" s="66"/>
+      <c r="F5" s="67" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="58"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="60"/>
+      <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="38">
@@ -3367,9 +3418,13 @@
       <c r="C8" s="13">
         <v>3.2</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="14">
+        <v>0.2</v>
+      </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="40"/>
+      <c r="F8" s="40">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="38">
@@ -3622,38 +3677,56 @@
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14">
-        <v>20.3</v>
+        <v>24.4</v>
       </c>
       <c r="F23" s="40">
-        <v>20.3</v>
+        <v>24.4</v>
       </c>
       <c r="G23" s="43"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
+      <c r="B24" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="40"/>
+      <c r="E24" s="14">
+        <v>6.3</v>
+      </c>
+      <c r="F24" s="40">
+        <v>6.3</v>
+      </c>
       <c r="G24" s="43"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
+      <c r="B25" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="14">
+        <v>16.5</v>
+      </c>
+      <c r="F25" s="40">
+        <v>16.5</v>
+      </c>
       <c r="G25" s="43"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="B26" s="22" t="s">
+        <v>77</v>
+      </c>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="44"/>
+      <c r="E26" s="25">
+        <v>9.5</v>
+      </c>
+      <c r="F26" s="44">
+        <v>9.5</v>
+      </c>
       <c r="G26" s="43"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3667,15 +3740,15 @@
       </c>
       <c r="D27" s="45">
         <f t="shared" ref="D27:F27" si="0">SUM(D7:D26)</f>
-        <v>43.100000000000009</v>
+        <v>43.300000000000004</v>
       </c>
       <c r="E27" s="45">
         <f t="shared" si="0"/>
-        <v>72.59</v>
+        <v>108.99</v>
       </c>
       <c r="F27" s="45">
         <f t="shared" si="0"/>
-        <v>166.39000000000001</v>
+        <v>205.79000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -3738,7 +3811,7 @@
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="2"/>
@@ -3749,7 +3822,7 @@
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
       <c r="E34" s="48">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="2"/>
@@ -3760,7 +3833,7 @@
       <c r="C35" s="48"/>
       <c r="D35" s="48">
         <f>D32*(E33/E34)</f>
-        <v>542500</v>
+        <v>708571.42857142852</v>
       </c>
       <c r="E35" s="48" t="s">
         <v>54</v>
@@ -3769,9 +3842,9 @@
         <v>10</v>
       </c>
       <c r="G35" s="2"/>
-      <c r="H35" s="64">
+      <c r="H35" s="53">
         <f>(D35/F35)</f>
-        <v>54250</v>
+        <v>70857.142857142855</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3782,7 +3855,7 @@
       <c r="B37" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="H37" s="66">
+      <c r="H37" s="55">
         <v>27000</v>
       </c>
     </row>
@@ -3791,36 +3864,161 @@
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="35"/>
-      <c r="H39" s="63">
+      <c r="H39" s="52">
         <f>(H35+H37)/4</f>
-        <v>20312.5</v>
+        <v>24464.285714285714</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="2"/>
+      <c r="C41" s="48"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="48"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="48">
+        <v>24556</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="48">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="48">
+        <f>350800*0.07</f>
+        <v>24556.000000000004</v>
+      </c>
+      <c r="D45" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="48">
+        <v>4</v>
+      </c>
+      <c r="F45" s="3">
+        <f>24556/4+200</f>
+        <v>6339</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="2"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="2"/>
+      <c r="C47" s="48"/>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="2"/>
+      <c r="C48" s="48"/>
+    </row>
+    <row r="49" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="48"/>
+    </row>
+    <row r="50" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="48">
+        <v>66000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="48">
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="2"/>
+      <c r="C52" s="48"/>
+    </row>
+    <row r="53" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="2"/>
+      <c r="C53" s="48"/>
+    </row>
+    <row r="54" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="2"/>
+      <c r="C54" s="48"/>
+    </row>
+    <row r="55" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="48"/>
+    </row>
+    <row r="56" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" s="48">
+        <v>2160</v>
+      </c>
+      <c r="D56" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="48">
+        <v>3813</v>
+      </c>
+      <c r="D57" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="48">
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="48">
+        <v>9493</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4292,17 +4490,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ad2e83f4-1684-48d1-85cc-3cc5bbc43bf0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72577035-6a57-4415-907e-65bfb8f4a467" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009F40A6B9DE1CF04FAD1F227B96E2F34C" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ebed63833b1c1ff8322ef47dcee476e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad2e83f4-1684-48d1-85cc-3cc5bbc43bf0" xmlns:ns3="72577035-6a57-4415-907e-65bfb8f4a467" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f86e976f22f91db45a78328c64c04444" ns2:_="" ns3:_="">
     <xsd:import namespace="ad2e83f4-1684-48d1-85cc-3cc5bbc43bf0"/>
@@ -4497,7 +4684,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4506,18 +4693,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{046CF1AA-3D8D-4BB5-BE2B-F24666DB68ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ad2e83f4-1684-48d1-85cc-3cc5bbc43bf0"/>
-    <ds:schemaRef ds:uri="72577035-6a57-4415-907e-65bfb8f4a467"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ad2e83f4-1684-48d1-85cc-3cc5bbc43bf0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72577035-6a57-4415-907e-65bfb8f4a467" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73EDA65F-DD11-48CA-A1BA-272ED93C4315}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4536,10 +4723,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE9170A3-9A57-4F8E-A2E8-3817A9C90B3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{046CF1AA-3D8D-4BB5-BE2B-F24666DB68ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ad2e83f4-1684-48d1-85cc-3cc5bbc43bf0"/>
+    <ds:schemaRef ds:uri="72577035-6a57-4415-907e-65bfb8f4a467"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>